<commit_message>
Add autofill for capstone ID
</commit_message>
<xml_diff>
--- a/Service/Reports/Capstone Projects 9-2-2020.xlsx
+++ b/Service/Reports/Capstone Projects 9-2-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\FinishedShopApp\venv\TempSource\Service\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D355F9-838D-45F1-B431-A439EC6701A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44930C1-A73F-47E3-B042-A8FEF85E3426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="23400" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capstone Projects 9-2-2020" sheetId="1" r:id="rId1"/>
@@ -1433,11 +1433,12 @@
   <dimension ref="A1:E134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="106.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>

</xml_diff>